<commit_message>
jsonjsdb_editor: dont update __mete__.json.js if no change
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb_editor/test/excel_version/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D891AD7D-520D-F042-ADE0-916F266FE690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5379863-42F0-CA41-9AA9-2B945E11D511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
jsonjsdb_editor : fixed : compare_datasets method skip entity starting with "__", refactored : use vite to bundle the lib and move compare_datasets in a separate file
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE57066-97E1-CE44-8484-4C793E481F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B082C9-5A7C-994B-8C95-7B4246BEDE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jsonjsdb_editor : fixed : prevent adding entry when old and new value are both null or empty
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA87B3-6CB1-6543-8206-7E9E83C1ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF60397-55A0-1643-B0B2-70948D093DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>bob 1</t>
+  </si>
+  <si>
+    <t>alice 333</t>
+  </si>
+  <si>
+    <t>folder_id</t>
+  </si>
+  <si>
+    <t>ok2</t>
   </si>
 </sst>
 </file>
@@ -443,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +473,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -479,7 +494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -492,8 +507,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -507,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -520,8 +538,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -535,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -548,13 +569,16 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>387</v>

</xml_diff>

<commit_message>
jsonjsdb_editor : changed : rename history to evolution
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF60397-55A0-1643-B0B2-70948D093DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F8B23-EEDB-2E47-984D-C65193AF123D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>alice 3</t>
   </si>
   <si>
-    <t>bob 3</t>
-  </si>
-  <si>
     <t>alice 1</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>ok2</t>
+  </si>
+  <si>
+    <t>bob 32</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,10 +474,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -561,7 +561,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>328</v>
@@ -578,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>387</v>

</xml_diff>